<commit_message>
Added generated features sheet to data dictionary
</commit_message>
<xml_diff>
--- a/data/data_dictionary.xlsx
+++ b/data/data_dictionary.xlsx
@@ -1,41 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholaspylypiw/Documents/GitHub/DS_Technical_Screen/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\demon\Documents\GitHub\cfc_ds_screen\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB5F4505-65E6-4B4E-A8DC-E799AE269846}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE38EC85-D02C-4470-A624-07FC10115CD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-3140" windowWidth="38400" windowHeight="21140" xr2:uid="{E6507000-19D6-3B4F-A9CD-9F10884C788D}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{E6507000-19D6-3B4F-A9CD-9F10884C788D}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Description" sheetId="1" r:id="rId1"/>
     <sheet name="RUCA Codes" sheetId="2" r:id="rId2"/>
+    <sheet name="Generated Features" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="111">
   <si>
     <t>dataset</t>
   </si>
@@ -362,13 +354,19 @@
   </si>
   <si>
     <t>Estimated percentage of households in tract with 2 or more vehicles</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>calculation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -428,6 +426,14 @@
       <color theme="1"/>
       <name val="Oswald Regular"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -656,7 +662,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -687,6 +693,7 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1010,18 +1017,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7D0361F-A881-194F-AD2B-8DE5EDEC5A63}">
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="26"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="26.25"/>
   <cols>
-    <col min="1" max="1" width="23.83203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="47.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="156.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="47.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="156.375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="38" thickBot="1">
+    <row r="1" spans="1:3" ht="27.75" thickBot="1">
       <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
@@ -1032,7 +1039,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="22">
+    <row r="2" spans="1:3" ht="18">
       <c r="A2" s="11" t="s">
         <v>3</v>
       </c>
@@ -1043,7 +1050,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="22">
+    <row r="3" spans="1:3" ht="18">
       <c r="A3" s="14" t="s">
         <v>3</v>
       </c>
@@ -1054,7 +1061,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="22">
+    <row r="4" spans="1:3" ht="18">
       <c r="A4" s="14" t="s">
         <v>3</v>
       </c>
@@ -1065,7 +1072,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="22">
+    <row r="5" spans="1:3" ht="18">
       <c r="A5" s="14" t="s">
         <v>3</v>
       </c>
@@ -1076,7 +1083,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="22">
+    <row r="6" spans="1:3" ht="18">
       <c r="A6" s="14" t="s">
         <v>3</v>
       </c>
@@ -1087,7 +1094,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="22">
+    <row r="7" spans="1:3" ht="18">
       <c r="A7" s="14" t="s">
         <v>3</v>
       </c>
@@ -1098,7 +1105,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="22">
+    <row r="8" spans="1:3" ht="18">
       <c r="A8" s="14" t="s">
         <v>3</v>
       </c>
@@ -1109,7 +1116,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="22">
+    <row r="9" spans="1:3" ht="18">
       <c r="A9" s="16" t="s">
         <v>16</v>
       </c>
@@ -1120,7 +1127,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="22">
+    <row r="10" spans="1:3" ht="18">
       <c r="A10" s="16" t="s">
         <v>16</v>
       </c>
@@ -1131,7 +1138,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="22">
+    <row r="11" spans="1:3" ht="18">
       <c r="A11" s="16" t="s">
         <v>16</v>
       </c>
@@ -1142,7 +1149,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="22">
+    <row r="12" spans="1:3" ht="18">
       <c r="A12" s="16" t="s">
         <v>16</v>
       </c>
@@ -1153,7 +1160,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="22">
+    <row r="13" spans="1:3" ht="18">
       <c r="A13" s="16" t="s">
         <v>16</v>
       </c>
@@ -1164,7 +1171,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="22">
+    <row r="14" spans="1:3" ht="18">
       <c r="A14" s="16" t="s">
         <v>16</v>
       </c>
@@ -1175,7 +1182,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="22">
+    <row r="15" spans="1:3" ht="18">
       <c r="A15" s="16" t="s">
         <v>16</v>
       </c>
@@ -1186,7 +1193,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="22">
+    <row r="16" spans="1:3" ht="18">
       <c r="A16" s="16" t="s">
         <v>16</v>
       </c>
@@ -1197,7 +1204,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="22">
+    <row r="17" spans="1:3" ht="18">
       <c r="A17" s="16" t="s">
         <v>16</v>
       </c>
@@ -1208,7 +1215,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="22">
+    <row r="18" spans="1:3" ht="18">
       <c r="A18" s="16" t="s">
         <v>16</v>
       </c>
@@ -1219,7 +1226,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="22">
+    <row r="19" spans="1:3" ht="18">
       <c r="A19" s="16" t="s">
         <v>16</v>
       </c>
@@ -1230,7 +1237,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="22">
+    <row r="20" spans="1:3" ht="18">
       <c r="A20" s="16" t="s">
         <v>16</v>
       </c>
@@ -1241,7 +1248,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="22">
+    <row r="21" spans="1:3" ht="18">
       <c r="A21" s="16" t="s">
         <v>16</v>
       </c>
@@ -1252,7 +1259,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="22">
+    <row r="22" spans="1:3" ht="18">
       <c r="A22" s="16" t="s">
         <v>16</v>
       </c>
@@ -1263,7 +1270,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="22">
+    <row r="23" spans="1:3" ht="18">
       <c r="A23" s="18" t="s">
         <v>44</v>
       </c>
@@ -1274,7 +1281,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="22">
+    <row r="24" spans="1:3" ht="18">
       <c r="A24" s="18" t="s">
         <v>44</v>
       </c>
@@ -1285,7 +1292,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="22">
+    <row r="25" spans="1:3" ht="18">
       <c r="A25" s="18" t="s">
         <v>44</v>
       </c>
@@ -1296,7 +1303,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="22">
+    <row r="26" spans="1:3" ht="18">
       <c r="A26" s="18" t="s">
         <v>44</v>
       </c>
@@ -1307,7 +1314,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="22">
+    <row r="27" spans="1:3" ht="18">
       <c r="A27" s="18" t="s">
         <v>44</v>
       </c>
@@ -1318,7 +1325,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="22">
+    <row r="28" spans="1:3" ht="18">
       <c r="A28" s="18" t="s">
         <v>44</v>
       </c>
@@ -1329,7 +1336,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="22">
+    <row r="29" spans="1:3" ht="18">
       <c r="A29" s="18" t="s">
         <v>44</v>
       </c>
@@ -1340,7 +1347,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="22">
+    <row r="30" spans="1:3" ht="18">
       <c r="A30" s="18" t="s">
         <v>44</v>
       </c>
@@ -1351,7 +1358,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="22">
+    <row r="31" spans="1:3" ht="18">
       <c r="A31" s="18" t="s">
         <v>44</v>
       </c>
@@ -1362,7 +1369,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="22">
+    <row r="32" spans="1:3" ht="18">
       <c r="A32" s="18" t="s">
         <v>44</v>
       </c>
@@ -1373,7 +1380,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="22">
+    <row r="33" spans="1:3" ht="18">
       <c r="A33" s="20" t="s">
         <v>83</v>
       </c>
@@ -1384,7 +1391,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="22">
+    <row r="34" spans="1:3" ht="18">
       <c r="A34" s="20" t="s">
         <v>83</v>
       </c>
@@ -1395,7 +1402,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="22">
+    <row r="35" spans="1:3" ht="18">
       <c r="A35" s="20" t="s">
         <v>83</v>
       </c>
@@ -1406,7 +1413,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="22">
+    <row r="36" spans="1:3" ht="18">
       <c r="A36" s="20" t="s">
         <v>83</v>
       </c>
@@ -1417,7 +1424,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="22">
+    <row r="37" spans="1:3" ht="18">
       <c r="A37" s="20" t="s">
         <v>83</v>
       </c>
@@ -1428,7 +1435,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="22">
+    <row r="38" spans="1:3" ht="18">
       <c r="A38" s="20" t="s">
         <v>83</v>
       </c>
@@ -1439,7 +1446,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="22">
+    <row r="39" spans="1:3" ht="18">
       <c r="A39" s="20" t="s">
         <v>83</v>
       </c>
@@ -1450,7 +1457,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="22">
+    <row r="40" spans="1:3" ht="18">
       <c r="A40" s="20" t="s">
         <v>83</v>
       </c>
@@ -1461,7 +1468,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="22">
+    <row r="41" spans="1:3" ht="18">
       <c r="A41" s="20" t="s">
         <v>83</v>
       </c>
@@ -1472,7 +1479,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="22">
+    <row r="42" spans="1:3" ht="18">
       <c r="A42" s="22" t="s">
         <v>100</v>
       </c>
@@ -1483,7 +1490,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="22">
+    <row r="43" spans="1:3" ht="18">
       <c r="A43" s="22" t="s">
         <v>100</v>
       </c>
@@ -1494,7 +1501,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="22">
+    <row r="44" spans="1:3" ht="18">
       <c r="A44" s="22" t="s">
         <v>100</v>
       </c>
@@ -1505,7 +1512,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="22">
+    <row r="45" spans="1:3" ht="18">
       <c r="A45" s="22" t="s">
         <v>100</v>
       </c>
@@ -1516,7 +1523,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="22">
+    <row r="46" spans="1:3" ht="18">
       <c r="A46" s="22" t="s">
         <v>100</v>
       </c>
@@ -1527,7 +1534,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="23" thickBot="1">
+    <row r="47" spans="1:3" ht="18.75" thickBot="1">
       <c r="A47" s="24" t="s">
         <v>100</v>
       </c>
@@ -1552,9 +1559,9 @@
       <selection sqref="A1:H46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="19">
+    <row r="1" spans="1:8" ht="18.75">
       <c r="A1" s="3" t="s">
         <v>60</v>
       </c>
@@ -1708,7 +1715,7 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:8" ht="19">
+    <row r="14" spans="1:8" ht="18.75">
       <c r="A14" s="3" t="s">
         <v>72</v>
       </c>
@@ -2149,4 +2156,36 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4567CBCD-0F7C-4CAF-B97D-382DA4C64B5B}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="2" max="2" width="35.25" customWidth="1"/>
+    <col min="3" max="3" width="95.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added generated features to dictionary
</commit_message>
<xml_diff>
--- a/data/data_dictionary.xlsx
+++ b/data/data_dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\demon\Documents\GitHub\cfc_ds_screen\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B130DE4-9ADE-4160-B97E-E62A8EF8577C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F753957-6AF1-45FE-B1EE-752DB982A0ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{E6507000-19D6-3B4F-A9CD-9F10884C788D}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="122">
   <si>
     <t>dataset</t>
   </si>
@@ -365,7 +365,34 @@
     <t>The average change in census/ACS tract population from 2010 to 2018</t>
   </si>
   <si>
-    <t>density</t>
+    <t>Estimated density for year 2018.</t>
+  </si>
+  <si>
+    <t>density_est_2018</t>
+  </si>
+  <si>
+    <t>groc14_per_capita</t>
+  </si>
+  <si>
+    <t>superc14_per_capita</t>
+  </si>
+  <si>
+    <t>convs14_per_capita</t>
+  </si>
+  <si>
+    <t>specs14_per_capita</t>
+  </si>
+  <si>
+    <t>Count of grocery stores in county 2014 per capita.</t>
+  </si>
+  <si>
+    <t>Count of supercenter stores in county 2014 per capita.</t>
+  </si>
+  <si>
+    <t>Count of convenience stores in county 2014 per capita.</t>
+  </si>
+  <si>
+    <t>Count of specialty food stores in county 2014 per capita.</t>
   </si>
 </sst>
 </file>
@@ -1023,8 +1050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7D0361F-A881-194F-AD2B-8DE5EDEC5A63}">
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="26.25"/>
@@ -1561,7 +1588,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D40778A4-F96B-0447-85E7-7F69ADF2143C}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
@@ -2164,11 +2193,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4567CBCD-0F7C-4CAF-B97D-382DA4C64B5B}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2195,7 +2224,42 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" t="s">
         <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated density description to 1,000 per capita
</commit_message>
<xml_diff>
--- a/data/data_dictionary.xlsx
+++ b/data/data_dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\demon\Documents\GitHub\cfc_ds_screen\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F753957-6AF1-45FE-B1EE-752DB982A0ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40C74CA6-C9AC-42DA-B2E4-24C5E474314F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{E6507000-19D6-3B4F-A9CD-9F10884C788D}"/>
   </bookViews>
@@ -371,28 +371,28 @@
     <t>density_est_2018</t>
   </si>
   <si>
-    <t>groc14_per_capita</t>
-  </si>
-  <si>
-    <t>superc14_per_capita</t>
-  </si>
-  <si>
-    <t>convs14_per_capita</t>
-  </si>
-  <si>
-    <t>specs14_per_capita</t>
-  </si>
-  <si>
-    <t>Count of grocery stores in county 2014 per capita.</t>
-  </si>
-  <si>
-    <t>Count of supercenter stores in county 2014 per capita.</t>
-  </si>
-  <si>
-    <t>Count of convenience stores in county 2014 per capita.</t>
-  </si>
-  <si>
-    <t>Count of specialty food stores in county 2014 per capita.</t>
+    <t>groc14_per_1k_capita</t>
+  </si>
+  <si>
+    <t>superc14_per_1k_capita</t>
+  </si>
+  <si>
+    <t>convs14_per_1k_capita</t>
+  </si>
+  <si>
+    <t>specs14_per_1k_capita</t>
+  </si>
+  <si>
+    <t>Count of grocery stores in county 2014 per 1,000 capita.</t>
+  </si>
+  <si>
+    <t>Count of supercenter stores in county 2014 per 1,000 capita.</t>
+  </si>
+  <si>
+    <t>Count of convenience stores in county 2014 per 1,000 capita.</t>
+  </si>
+  <si>
+    <t>Count of specialty food stores in county 2014 per 1,000 capita.</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Updated density per square mile
</commit_message>
<xml_diff>
--- a/data/data_dictionary.xlsx
+++ b/data/data_dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\demon\Documents\GitHub\cfc_ds_screen\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40C74CA6-C9AC-42DA-B2E4-24C5E474314F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1E028B-60C8-48E8-B879-36FB2430F244}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{E6507000-19D6-3B4F-A9CD-9F10884C788D}"/>
   </bookViews>
@@ -365,12 +365,6 @@
     <t>The average change in census/ACS tract population from 2010 to 2018</t>
   </si>
   <si>
-    <t>Estimated density for year 2018.</t>
-  </si>
-  <si>
-    <t>density_est_2018</t>
-  </si>
-  <si>
     <t>groc14_per_1k_capita</t>
   </si>
   <si>
@@ -393,6 +387,12 @@
   </si>
   <si>
     <t>Count of specialty food stores in county 2014 per 1,000 capita.</t>
+  </si>
+  <si>
+    <t>pop_1k_per_sqmi_est_2018</t>
+  </si>
+  <si>
+    <t>Estimated density of tract at 1,000 people per square mile estimate at year 2018.</t>
   </si>
 </sst>
 </file>
@@ -1050,8 +1050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7D0361F-A881-194F-AD2B-8DE5EDEC5A63}">
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="26.25"/>
@@ -1589,7 +1589,7 @@
   <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2197,7 +2197,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2224,42 +2224,42 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated density variable for interpretation
</commit_message>
<xml_diff>
--- a/data/data_dictionary.xlsx
+++ b/data/data_dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\demon\Documents\GitHub\cfc_ds_screen\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1E028B-60C8-48E8-B879-36FB2430F244}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08E6DE4-6C6D-4A26-B4E2-A0D2D974C57B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{E6507000-19D6-3B4F-A9CD-9F10884C788D}"/>
   </bookViews>
@@ -389,10 +389,10 @@
     <t>Count of specialty food stores in county 2014 per 1,000 capita.</t>
   </si>
   <si>
-    <t>pop_1k_per_sqmi_est_2018</t>
-  </si>
-  <si>
-    <t>Estimated density of tract at 1,000 people per square mile estimate at year 2018.</t>
+    <t>log_pop_per_sqmi_est_2018</t>
+  </si>
+  <si>
+    <t>Estimated log10 density of tract - log10 people per square mile estimate at year 2018.</t>
   </si>
 </sst>
 </file>
@@ -2197,7 +2197,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
Added univariate logistic modeling for feature selection
</commit_message>
<xml_diff>
--- a/data/data_dictionary.xlsx
+++ b/data/data_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\demon\Documents\GitHub\cfc_ds_screen\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08E6DE4-6C6D-4A26-B4E2-A0D2D974C57B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ABD0831-2F31-4516-981E-9F8E96B9C3C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{E6507000-19D6-3B4F-A9CD-9F10884C788D}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{E6507000-19D6-3B4F-A9CD-9F10884C788D}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Description" sheetId="1" r:id="rId1"/>
@@ -1050,7 +1050,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7D0361F-A881-194F-AD2B-8DE5EDEC5A63}">
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
@@ -2195,7 +2195,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4567CBCD-0F7C-4CAF-B97D-382DA4C64B5B}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>

</xml_diff>